<commit_message>
CV_esp full version with LaTeX code in vitae::detailed_entries
</commit_message>
<xml_diff>
--- a/data/award_es.xlsx
+++ b/data/award_es.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF1018D-53A8-4760-9C6E-7AA3C9452124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75D3673-637B-4154-8B09-5FFE5E0C1B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28515" yWindow="7965" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28470" yWindow="1470" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -37,18 +37,12 @@
     <t>why</t>
   </si>
   <si>
-    <t>Universidad El Bosque</t>
-  </si>
-  <si>
     <t>Grindley Grants</t>
   </si>
   <si>
     <t>Sep. 2014</t>
   </si>
   <si>
-    <t>Experimental Psychology Society</t>
-  </si>
-  <si>
     <t>Oct. 2010 - Oct. 2014</t>
   </si>
   <si>
@@ -58,21 +52,12 @@
     <t>Oct. 2009</t>
   </si>
   <si>
-    <t>School of Life Sciences – University of Liverpool</t>
-  </si>
-  <si>
     <t>University of Liverpool International Scholarship</t>
   </si>
   <si>
     <t>Sep. 2008 - Sep. 2009</t>
   </si>
   <si>
-    <t>University of Liverpool</t>
-  </si>
-  <si>
-    <t>Colfuturo</t>
-  </si>
-  <si>
     <t>Dic. 2018</t>
   </si>
   <si>
@@ -82,12 +67,6 @@
     <t>Dic. 2019</t>
   </si>
   <si>
-    <t>COP$5.000.000</t>
-  </si>
-  <si>
-    <t>COP$7.000.000</t>
-  </si>
-  <si>
     <t>Programa Crédito-Beca</t>
   </si>
   <si>
@@ -115,31 +94,52 @@
     <t>Sep. 2020</t>
   </si>
   <si>
-    <t>Ig Nobel Prize</t>
-  </si>
-  <si>
     <t>Economics Prize</t>
   </si>
   <si>
     <t>Mejor desempeño general en la maestría</t>
   </si>
   <si>
-    <t>Minciencias</t>
-  </si>
-  <si>
     <t>IX Convocatoria de Estímulos a la Excelencia</t>
   </si>
   <si>
     <t>Dic. 2022</t>
   </si>
   <si>
-    <t>COP$10.000.000</t>
-  </si>
-  <si>
     <t>Cambridge, MA, EE.UU.</t>
   </si>
   <si>
-    <t>Por ‘tratar de cuantificar la relación entre la desigualdad de ingresos nacionales en diferentes países y la cantidad promedio de besos boca a boca’ (Watkins, et al., 2019)</t>
+    <t>\href{https://www.unbosque.edu.co/}{Universidad El Bosque}</t>
+  </si>
+  <si>
+    <t>\href{https://minciencias.gov.co/}{Minciencias}</t>
+  </si>
+  <si>
+    <t>\href{https://eps.ac.uk/}{Experimental Psychology Society}</t>
+  </si>
+  <si>
+    <t>\href{https://www.liverpool.ac.uk/life-sciences/}{School of Life Sciences} – University of Liverpool</t>
+  </si>
+  <si>
+    <t>\href{https://www.liverpool.ac.uk/}{University of Liverpool}</t>
+  </si>
+  <si>
+    <t>\href{https://www.colfuturo.org/}{Colfuturo}</t>
+  </si>
+  <si>
+    <t>\href{https://improbable.com/ig/about-the-ig-nobel-prizes/}{Ig Nobel Prize}</t>
+  </si>
+  <si>
+    <t>Por ‘tratar de cuantificar la relación entre la desigualdad de ingresos nacionales en diferentes países y la cantidad promedio de besos boca a boca’ (\href{https://doi.org/10.1038/s41598-019-43267-7}{Watkins, et al., 2019})</t>
+  </si>
+  <si>
+    <t>COP\$10.000.000</t>
+  </si>
+  <si>
+    <t>COP\$7.000.000</t>
+  </si>
+  <si>
+    <t>COP\$5.000.000</t>
   </si>
 </sst>
 </file>
@@ -634,12 +634,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -996,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,176 +1017,192 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1" t="s">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="E11" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>